<commit_message>
latest updates in read me
</commit_message>
<xml_diff>
--- a/factors_dataset.xlsx
+++ b/factors_dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Dropbox (Lehigh University)\Postdoc_Lehigh\Teaching\ISE321 - OutreachISE - Ana I. Alexandrescu\Code\Factors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Lehigh University Dropbox\Tommaso Giovannelli\Postdoc_Lehigh\Teaching\ISE321 - OutreachISE - Ana I. Alexandrescu\Code\JournalSportsAnalytics\Rev1\Factors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0017A3-F33E-45F0-8024-4609F108D5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65FFFC6-D996-4017-9FFF-9456AFD91519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3984" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseNormalized" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Sports</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Ball velocity</t>
-  </si>
-  <si>
-    <t>Ball geometry</t>
   </si>
   <si>
     <t>Ball bounciness</t>
@@ -446,50 +443,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2108E0F-AB6E-464C-ADAA-1AE693FE742F}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
         <v>15</v>
       </c>
       <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
       </c>
       <c r="F1" t="s">
         <v>16</v>
       </c>
       <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
       <c r="I1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="J1" t="s">
         <v>23</v>
       </c>
       <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
         <v>24</v>
-      </c>
-      <c r="L1" t="s">
-        <v>19</v>
       </c>
       <c r="M1" t="s">
         <v>25</v>
@@ -498,13 +495,10 @@
         <v>26</v>
       </c>
       <c r="O1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -521,40 +515,37 @@
         <v>0.1884158735</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="G2">
-        <v>0.8</v>
+        <v>9.3192585500000008E-3</v>
       </c>
       <c r="H2">
-        <v>9.3192585500000008E-3</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0.90785447129999997</v>
       </c>
       <c r="J2">
-        <v>0.90785447129999997</v>
+        <v>8.3333333329999995E-2</v>
       </c>
       <c r="K2">
-        <v>8.3333333329999995E-2</v>
+        <v>9.5680480689999993E-3</v>
       </c>
       <c r="L2">
-        <v>9.5680480689999993E-3</v>
+        <v>1</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
       <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>0.16666666669999999</v>
-      </c>
-      <c r="P2" s="1">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.23519999999999999</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -571,40 +562,37 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0.27021674769999998</v>
       </c>
       <c r="H3">
-        <v>0.27021674769999998</v>
+        <v>5.6773805949999999E-2</v>
       </c>
       <c r="I3">
-        <v>5.6773805949999999E-2</v>
+        <v>0.80176810610000004</v>
       </c>
       <c r="J3">
-        <v>0.80176810610000004</v>
+        <v>0.25</v>
       </c>
       <c r="K3">
-        <v>0.25</v>
+        <v>0.29730097700000002</v>
       </c>
       <c r="L3">
-        <v>0.29730097700000002</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0.16666666669999999</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.23519999999999999</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -621,40 +609,37 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="G4">
-        <v>0.6</v>
+        <v>2.0497378430000001E-2</v>
       </c>
       <c r="H4">
-        <v>2.0497378430000001E-2</v>
+        <v>0.1889456293</v>
       </c>
       <c r="I4">
-        <v>0.1889456293</v>
+        <v>0.65028901729999999</v>
       </c>
       <c r="J4">
-        <v>0.65028901729999999</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0.74962673710000005</v>
       </c>
       <c r="M4">
-        <v>0.74962673710000005</v>
+        <v>0.58996876980000001</v>
       </c>
       <c r="N4">
-        <v>0.58996876980000001</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -671,40 +656,37 @@
         <v>7.3589632749999995E-2</v>
       </c>
       <c r="F5">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="G5">
-        <v>0.7</v>
+        <v>0.43093671030000003</v>
       </c>
       <c r="H5">
-        <v>0.43093671030000003</v>
+        <v>5.6773805949999999E-2</v>
       </c>
       <c r="I5">
-        <v>5.6773805949999999E-2</v>
+        <v>0.94282799829999997</v>
       </c>
       <c r="J5">
-        <v>0.94282799829999997</v>
+        <v>0.6</v>
       </c>
       <c r="K5">
-        <v>0.6</v>
+        <v>0.2218047507</v>
       </c>
       <c r="L5">
-        <v>0.2218047507</v>
+        <v>2.360990336E-2</v>
       </c>
       <c r="M5">
-        <v>2.360990336E-2</v>
+        <v>0.81891187450000003</v>
       </c>
       <c r="N5">
-        <v>0.81891187450000003</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5" s="1">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -724,37 +706,34 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>0.48612963770000001</v>
       </c>
       <c r="H6">
-        <v>0.48612963770000001</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>0.79054743279999995</v>
       </c>
       <c r="J6">
-        <v>0.79054743279999995</v>
+        <v>0.90833333329999999</v>
       </c>
       <c r="K6">
-        <v>0.90833333329999999</v>
+        <v>7.8757422830000007E-2</v>
       </c>
       <c r="L6">
-        <v>7.8757422830000007E-2</v>
+        <v>9.8426553350000001E-2</v>
       </c>
       <c r="M6">
-        <v>9.8426553350000001E-2</v>
+        <v>0.99149975339999996</v>
       </c>
       <c r="N6">
-        <v>0.99149975339999996</v>
-      </c>
-      <c r="O6">
-        <v>0.41666666670000002</v>
-      </c>
-      <c r="P6" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+        <v>0.58819999999999995</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -771,10 +750,10 @@
         <v>6.6003117949999995E-2</v>
       </c>
       <c r="F7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G7">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -783,28 +762,25 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>0.55066666669999997</v>
       </c>
       <c r="K7">
-        <v>0.55066666669999997</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>7.280656311E-2</v>
       </c>
       <c r="M7">
-        <v>7.280656311E-2</v>
+        <v>0.82969450769999997</v>
       </c>
       <c r="N7">
-        <v>0.82969450769999997</v>
-      </c>
-      <c r="O7">
-        <v>0.53333333329999999</v>
-      </c>
-      <c r="P7" s="1">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.75290000000000001</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -821,40 +797,37 @@
         <v>0.1264806067</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="G8">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0.32412135780000001</v>
       </c>
       <c r="I8">
-        <v>0.32412135780000001</v>
+        <v>1</v>
       </c>
       <c r="J8">
         <v>1</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>2.8825889220000001E-2</v>
       </c>
       <c r="L8">
-        <v>2.8825889220000001E-2</v>
+        <v>3.8704490639999999E-2</v>
       </c>
       <c r="M8">
-        <v>3.8704490639999999E-2</v>
+        <v>0.92810012450000001</v>
       </c>
       <c r="N8">
-        <v>0.92810012450000001</v>
-      </c>
-      <c r="O8">
-        <v>0.66666666669999997</v>
-      </c>
-      <c r="P8" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.94110000000000005</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -871,40 +844,37 @@
         <v>6.2224028930000001E-2</v>
       </c>
       <c r="F9">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="G9">
-        <v>0.7</v>
+        <v>0.1934746007</v>
       </c>
       <c r="H9">
-        <v>0.1934746007</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0.84665079899999995</v>
       </c>
       <c r="J9">
-        <v>0.84665079899999995</v>
+        <v>0.68666666669999998</v>
       </c>
       <c r="K9">
-        <v>0.68666666669999998</v>
+        <v>0.15302808379999999</v>
       </c>
       <c r="L9">
-        <v>0.15302808379999999</v>
+        <v>0.31893878489999999</v>
       </c>
       <c r="M9">
-        <v>0.31893878489999999</v>
+        <v>0.94923333409999999</v>
       </c>
       <c r="N9">
-        <v>0.94923333409999999</v>
-      </c>
-      <c r="O9">
-        <v>0.53333333329999999</v>
-      </c>
-      <c r="P9" s="1">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.75290000000000001</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -924,37 +894,34 @@
         <v>0.5</v>
       </c>
       <c r="G10">
+        <v>0.46265483470000002</v>
+      </c>
+      <c r="H10">
+        <v>5.6773805949999999E-2</v>
+      </c>
+      <c r="I10">
+        <v>0.94282799829999997</v>
+      </c>
+      <c r="J10">
         <v>0.5</v>
       </c>
-      <c r="H10">
-        <v>0.46265483470000002</v>
-      </c>
-      <c r="I10">
-        <v>5.6773805949999999E-2</v>
-      </c>
-      <c r="J10">
-        <v>0.94282799829999997</v>
-      </c>
       <c r="K10">
-        <v>0.5</v>
+        <v>0.30204419539999999</v>
       </c>
       <c r="L10">
-        <v>0.30204419539999999</v>
+        <v>0.1294360859</v>
       </c>
       <c r="M10">
-        <v>0.1294360859</v>
+        <v>0.77488435440000003</v>
       </c>
       <c r="N10">
-        <v>0.77488435440000003</v>
-      </c>
-      <c r="O10">
-        <v>0.3</v>
-      </c>
-      <c r="P10" s="1">
+        <v>0.42349999999999999</v>
+      </c>
+      <c r="O10" s="1">
         <v>0.37</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -971,40 +938,37 @@
         <v>0.43310908799999998</v>
       </c>
       <c r="F11">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="G11">
-        <v>0.9</v>
+        <v>1.16709776E-2</v>
       </c>
       <c r="H11">
-        <v>1.16709776E-2</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>0.93641618500000001</v>
       </c>
       <c r="J11">
-        <v>0.93641618500000001</v>
+        <v>0.91666666669999997</v>
       </c>
       <c r="K11">
-        <v>0.91666666669999997</v>
+        <v>3.11058107E-2</v>
       </c>
       <c r="L11">
-        <v>3.11058107E-2</v>
+        <v>0.1666992075</v>
       </c>
       <c r="M11">
-        <v>0.1666992075</v>
+        <v>0.92457792279999995</v>
       </c>
       <c r="N11">
-        <v>0.92457792279999995</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
         <v>0.08</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1021,40 +985,37 @@
         <v>0.1635711182</v>
       </c>
       <c r="F12">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G12">
-        <v>0.1</v>
+        <v>0.258999223</v>
       </c>
       <c r="H12">
-        <v>0.258999223</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>0.81859911590000001</v>
       </c>
       <c r="J12">
-        <v>0.81859911590000001</v>
+        <v>0.91666666669999997</v>
       </c>
       <c r="K12">
-        <v>0.91666666669999997</v>
+        <v>0.12318696799999999</v>
       </c>
       <c r="L12">
-        <v>0.12318696799999999</v>
+        <v>7.6892155739999996E-2</v>
       </c>
       <c r="M12">
-        <v>7.6892155739999996E-2</v>
+        <v>0.92810012450000001</v>
       </c>
       <c r="N12">
-        <v>0.92810012450000001</v>
-      </c>
-      <c r="O12">
-        <v>1</v>
-      </c>
-      <c r="P12" s="1">
+        <v>1</v>
+      </c>
+      <c r="O12" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1071,37 +1032,34 @@
         <v>0.79161633389999997</v>
       </c>
       <c r="F13">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="G13">
+        <v>1.16709776E-2</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0.91805508329999996</v>
+      </c>
+      <c r="J13">
+        <v>0.88583333330000003</v>
+      </c>
+      <c r="K13">
+        <v>4.1284812130000001E-2</v>
+      </c>
+      <c r="L13">
+        <v>0.4240266452</v>
+      </c>
+      <c r="M13">
+        <v>0.98163758889999997</v>
+      </c>
+      <c r="N13">
+        <v>0.23519999999999999</v>
+      </c>
+      <c r="O13" s="1">
         <v>0.3</v>
-      </c>
-      <c r="H13">
-        <v>1.16709776E-2</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0.91805508329999996</v>
-      </c>
-      <c r="K13">
-        <v>0.88583333330000003</v>
-      </c>
-      <c r="L13">
-        <v>4.1284812130000001E-2</v>
-      </c>
-      <c r="M13">
-        <v>0.4240266452</v>
-      </c>
-      <c r="N13">
-        <v>0.98163758889999997</v>
-      </c>
-      <c r="O13">
-        <v>0.16666666669999999</v>
-      </c>
-      <c r="P13" s="1">
-        <v>0.31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>